<commit_message>
Updated script with data from last season (Dryad)
</commit_message>
<xml_diff>
--- a/output/seasonal_stats.xlsx
+++ b/output/seasonal_stats.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>season</t>
   </si>
@@ -59,6 +59,9 @@
   </si>
   <si>
     <t>M2_08 Draconid 2020</t>
+  </si>
+  <si>
+    <t>M2_09 Dryad 2020</t>
   </si>
 </sst>
 </file>
@@ -416,7 +419,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -653,6 +656,32 @@
         <v>10246</v>
       </c>
     </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="1">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10">
+        <v>9678</v>
+      </c>
+      <c r="D10">
+        <v>10725</v>
+      </c>
+      <c r="E10">
+        <v>855528</v>
+      </c>
+      <c r="F10">
+        <v>9946</v>
+      </c>
+      <c r="G10">
+        <v>10046</v>
+      </c>
+      <c r="H10">
+        <v>10183</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update stats new season
</commit_message>
<xml_diff>
--- a/output/seasonal_stats.xlsx
+++ b/output/seasonal_stats.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>season</t>
   </si>
@@ -62,6 +62,9 @@
   </si>
   <si>
     <t>M2_09 Dryad 2020</t>
+  </si>
+  <si>
+    <t>M2_10 Cat 2020</t>
   </si>
 </sst>
 </file>
@@ -419,7 +422,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -670,7 +673,7 @@
         <v>10725</v>
       </c>
       <c r="E10">
-        <v>855528</v>
+        <v>854877</v>
       </c>
       <c r="F10">
         <v>9946</v>
@@ -680,6 +683,32 @@
       </c>
       <c r="H10">
         <v>10183</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11">
+        <v>9703</v>
+      </c>
+      <c r="D11">
+        <v>10804</v>
+      </c>
+      <c r="E11">
+        <v>929613</v>
+      </c>
+      <c r="F11">
+        <v>9977</v>
+      </c>
+      <c r="G11">
+        <v>10067</v>
+      </c>
+      <c r="H11">
+        <v>10176</v>
       </c>
     </row>
   </sheetData>

</xml_diff>